<commit_message>
Update one function in part3.py
</commit_message>
<xml_diff>
--- a/Tasks_Table.xlsx
+++ b/Tasks_Table.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swchak/Desktop/Vrije Universiteit Amsterdam/1_BA/Year 2_2024-2025/Semester 2/P4_Data Engineering/Assignments/Group/Flight_DataEngineering/__pycache__/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swchak/Desktop/Vrije Universiteit Amsterdam/1_BA/Year 2_2024-2025/Semester 2/P4_Data Engineering/Assignments/Group/Flight_DataEngineering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F112B84-84EF-FF4A-AAD3-2FDF7CC30D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFDDB4D-6281-5140-AF7D-85A13C81A625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16180" xr2:uid="{31F3B9D3-5FC3-B44C-9B59-F8837806067A}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16100" xr2:uid="{31F3B9D3-5FC3-B44C-9B59-F8837806067A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t xml:space="preserve">Set up a map of the world with points on it indicating the airports in the set. </t>
   </si>
@@ -80,9 +80,6 @@
     <t>Write a function that computes the inner product between the flight direction and the wind speed of a given flight.</t>
   </si>
   <si>
-    <t xml:space="preserve"> The wind direction is given in weather in degrees. Compute for each airport the direction the plane follows when flying there from New York.</t>
-  </si>
-  <si>
     <t>Is there a relation between the sign of this inner product and the air time?</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
   </si>
   <si>
     <t>File</t>
-  </si>
-  <si>
-    <t>part1.py</t>
   </si>
   <si>
     <t>drawLine()</t>
@@ -161,9 +155,6 @@
     <t>departureDelayPlot()</t>
   </si>
   <si>
-    <t>arrivalDelayPlot():</t>
-  </si>
-  <si>
     <t>amongOfDelayFlights()</t>
   </si>
   <si>
@@ -192,13 +183,46 @@
   </si>
   <si>
     <t>Cannot think of a proper title 🫠</t>
+  </si>
+  <si>
+    <t>Check the table flights for missing values think of ways to resolve them.</t>
+  </si>
+  <si>
+    <t>Write a function that checks whether the data in   is in order. That is, verify that the air time , dep time ,   etc. match for each flight. If not, think of ways to resolve it if this is not the case.</t>
+  </si>
+  <si>
+    <t>Convert the (schedueled and actual) arrival departure and departure moments to datetime objects.</t>
+  </si>
+  <si>
+    <t>Create a column that contains the local arrival time, incorporating the time difference between arrival and departure airport.</t>
+  </si>
+  <si>
+    <t>In addition, information on the different types of planes and airlines will be important. Consider studying what the effect of the wind or precipitation is on different plane types.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The dashboard will also contain a general results tab that can show anything you find remarkable in the data. Think of things you would like to display here. Are there interesting relations to be seen in the data? Are there airports that stand out when it comes to delay? Are there plane times that fly considerable faster? Which plane routes are taken most often from NYC? Is there a significant relation between (some) weather variables and the delay time? Come up with convincing graphical or numerical summaries that can be displayed in this part of the dashboard to display the results of the study. </t>
+  </si>
+  <si>
+    <t>Next week, the specifics of the dashboard will be released. Count on requirements asking for the statistics for different departure and arrival airports. Consider making functions that take these airports as input and generate numerical or graphical representations of the data grouped by them. Many of the tasks from the previous parts can be grouped!</t>
+  </si>
+  <si>
+    <t>arrivalDelayPlot()</t>
+  </si>
+  <si>
+    <t>Look for duplicates in the flights table. Take into account that here a flight number can occur multiple times, only count it as duplicate when the same flight appears multiple times.</t>
+  </si>
+  <si>
+    <t>The wind direction is given in weather in degrees. Compute for each airport the direction the plane follows when flying there from New York.</t>
+  </si>
+  <si>
+    <t>compute_wind_direction_from_NYC()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -239,6 +263,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="CMR10"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -254,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -271,11 +300,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -304,11 +392,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -366,236 +472,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -937,13 +813,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F4BD72-E2E4-3344-B69D-5B019EDA64B4}">
-  <dimension ref="A1:J27"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C16"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="89.83203125" style="1" customWidth="1"/>
@@ -957,29 +834,29 @@
     <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="20">
       <c r="A1" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -990,10 +867,10 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="I4" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1003,21 +880,21 @@
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="I5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="1">
-        <f>COUNTIF(F$4:F$26,$I5)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="14">
+        <f>COUNTIF(F$4:F$35,$I5)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1029,21 +906,21 @@
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="I6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="1">
-        <f t="shared" ref="J6:J7" si="0">COUNTIF(F$4:F$26,$I6)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="I6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="11">
+        <f t="shared" ref="J6:J7" si="0">COUNTIF(F$4:F$35,$I6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -1053,25 +930,23 @@
       <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="I7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="I7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="15">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -1081,14 +956,14 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="30">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1098,14 +973,14 @@
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="30">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -1115,14 +990,14 @@
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="30">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1132,14 +1007,14 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="45">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -1150,11 +1025,11 @@
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -1165,188 +1040,190 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="51">
       <c r="A14" s="1">
         <v>1</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="51">
       <c r="A15" s="1">
         <v>2</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="34">
       <c r="A16" s="1">
         <v>3</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="34">
       <c r="A17" s="1">
         <v>4</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="68">
       <c r="A18" s="1">
         <v>5</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="34">
       <c r="A19" s="1">
         <v>6</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="34">
       <c r="A20" s="1">
         <v>7</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="34">
       <c r="A21" s="1">
         <v>8</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="17">
       <c r="A22" s="1">
         <v>9</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="51">
       <c r="A23" s="1">
         <v>10</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="34">
       <c r="A24" s="1">
         <v>11</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
+      <c r="E24" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="F24" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="34">
       <c r="A25" s="1">
         <v>12</v>
       </c>
@@ -1357,28 +1234,28 @@
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>13</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1387,31 +1264,151 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
+    <row r="28" spans="1:7" ht="17">
+      <c r="A28" s="1">
+        <v>1</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="1:7" ht="34">
+      <c r="A29" s="1">
+        <v>2</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="9"/>
+    </row>
+    <row r="30" spans="1:7" ht="17">
+      <c r="A30" s="1">
+        <v>3</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="1:7" ht="34">
+      <c r="A31" s="1">
+        <v>4</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31" s="9"/>
+    </row>
+    <row r="32" spans="1:7" ht="34">
+      <c r="A32" s="1">
+        <v>5</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32" s="9"/>
+    </row>
+    <row r="33" spans="1:7" ht="34">
+      <c r="A33" s="1">
+        <v>6</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" s="9"/>
+    </row>
+    <row r="34" spans="1:7" ht="68">
+      <c r="A34" s="1">
+        <v>7</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="1:7" ht="90">
+      <c r="A35" s="1">
+        <v>8</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="9"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:G26">
-    <cfRule type="expression" dxfId="5" priority="7">
+  <conditionalFormatting sqref="A5:G35">
+    <cfRule type="expression" dxfId="5" priority="10">
       <formula>$F5=$I$7</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>$F5=$I$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="10">
+    <cfRule type="expression" dxfId="3" priority="13">
       <formula>$F5=$I$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:I7">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$I5=$I$7</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>$I5=$I$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>$I5=$I$5</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F12 F14:F26" xr:uid="{9ECECD3F-B10C-D446-A358-3A7D162D644C}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F12 F14:F26 F28:F35" xr:uid="{9ECECD3F-B10C-D446-A358-3A7D162D644C}">
       <formula1>$I$5:$I$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update a few functions
</commit_message>
<xml_diff>
--- a/Tasks_Table.xlsx
+++ b/Tasks_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swchak/Desktop/Vrije Universiteit Amsterdam/1_BA/Year 2_2024-2025/Semester 2/P4_Data Engineering/Assignments/Group/Flight_DataEngineering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFDDB4D-6281-5140-AF7D-85A13C81A625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50812406-9A36-6E48-8C96-07E9D30D2E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16100" xr2:uid="{31F3B9D3-5FC3-B44C-9B59-F8837806067A}"/>
+    <workbookView xWindow="4360" yWindow="520" windowWidth="24460" windowHeight="16100" xr2:uid="{31F3B9D3-5FC3-B44C-9B59-F8837806067A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
   <si>
     <t xml:space="preserve">Set up a map of the world with points on it indicating the airports in the set. </t>
   </si>
@@ -89,20 +89,10 @@
     <t>Function</t>
   </si>
   <si>
-    <t>File</t>
-  </si>
-  <si>
     <t>drawLine()</t>
   </si>
   <si>
     <t>drawMultipleLines()</t>
-  </si>
-  <si>
-    <t>Verify that the distances you computed in part 1 are roughly equal to the dis- tances in the variable distance in the table flights . If they are much off, recall that latitude and longitude represent angles expressed in degrees, while the functions sin and cos expects entries in radial angles.</t>
-  </si>
-  <si>
-    <t>For each flight, the origin from which it leaves can be fount in the variable origin in the table . Identify all different airports in NYC from which flights depart and save a contain the information about those
-airports from airports</t>
   </si>
   <si>
     <t>Write a function that takes a month and day and an airport in NYC as input,
@@ -188,9 +178,6 @@
     <t>Check the table flights for missing values think of ways to resolve them.</t>
   </si>
   <si>
-    <t>Write a function that checks whether the data in   is in order. That is, verify that the air time , dep time ,   etc. match for each flight. If not, think of ways to resolve it if this is not the case.</t>
-  </si>
-  <si>
     <t>Convert the (schedueled and actual) arrival departure and departure moments to datetime objects.</t>
   </si>
   <si>
@@ -216,6 +203,54 @@
   </si>
   <si>
     <t>compute_wind_direction_from_NYC()</t>
+  </si>
+  <si>
+    <t>drop_duplicates_except()</t>
+  </si>
+  <si>
+    <t>check_na_flights()</t>
+  </si>
+  <si>
+    <t>convert_datetime()</t>
+  </si>
+  <si>
+    <t>Write a function that checks whether the data in flights is in order. That is, verify that the air_time , dep _ime ,  sched_dep_time etc. match for each flight. If not, think of ways to resolve it if this is not the case.</t>
+  </si>
+  <si>
+    <t>local_arrival_time()</t>
+  </si>
+  <si>
+    <t>Problems</t>
+  </si>
+  <si>
+    <t>Running time is too slow</t>
+  </si>
+  <si>
+    <t>The result of should be verified</t>
+  </si>
+  <si>
+    <t>The result of should be verified (not sure about are the distances calculated in correct unit)</t>
+  </si>
+  <si>
+    <t>Do not know what the inner product should be</t>
+  </si>
+  <si>
+    <t>The result of should be verified (not sure about the calculation of angle is correct or not)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Verify that the distances you computed in part 1 are roughly equal to the distances in the variable distance in the table flights . If they are much off, recall that latitude and longitude represent angles expressed in degrees, while the functions sin and cos expects entries in radial angles.</t>
+  </si>
+  <si>
+    <t>No function is used to verified</t>
+  </si>
+  <si>
+    <t>For each flight, the origin from which it leaves can be found in the variable origin in the table . Identify all different airports in NYC from which flights depart and save a DataFrame contain the information about those airports from airports</t>
+  </si>
+  <si>
+    <t>unique_depart_airports()</t>
   </si>
 </sst>
 </file>
@@ -283,7 +318,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -359,11 +394,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -408,6 +471,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -816,19 +885,19 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="89.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="1"/>
     <col min="9" max="9" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="1"/>
@@ -836,7 +905,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20">
       <c r="A1" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -844,16 +913,16 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -867,7 +936,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="I4" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -878,23 +947,23 @@
         <v>0</v>
       </c>
       <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="E5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="I5" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J5" s="14">
-        <f>COUNTIF(F$4:F$35,$I5)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <f>COUNTIF(E$4:E$35,$I5)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -904,23 +973,23 @@
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="E6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J6" s="11">
-        <f t="shared" ref="J6:J7" si="0">COUNTIF(F$4:F$35,$I6)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="30">
+        <f>COUNTIF(E$4:E$35,$I6)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -930,20 +999,20 @@
       <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="E7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="I7" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J7" s="15">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f>COUNTIF(E$4:E$35,$I7)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30">
@@ -954,16 +1023,23 @@
         <v>1</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:10" ht="30">
+      <c r="I8" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="17">
+        <f>SUM(J5:J7)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="34">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -971,12 +1047,14 @@
         <v>5</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="E9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="G9" s="9"/>
     </row>
@@ -988,12 +1066,14 @@
         <v>6</v>
       </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="E10" s="9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="G10" s="9"/>
     </row>
@@ -1005,13 +1085,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="E11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F11" s="9"/>
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:10" ht="45">
@@ -1023,10 +1103,10 @@
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="E12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="9"/>
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:10">
@@ -1045,29 +1125,33 @@
         <v>1</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="E14" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="F14" s="9" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:10" ht="51">
+    <row r="15" spans="1:10" ht="34">
       <c r="A15" s="1">
         <v>2</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="D15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="9"/>
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:10" ht="34">
@@ -1075,16 +1159,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="E16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F16" s="9"/>
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" ht="34">
@@ -1092,33 +1176,33 @@
         <v>4</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="E17" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" ht="68">
+    <row r="18" spans="1:7" ht="51">
       <c r="A18" s="1">
         <v>5</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="E18" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" ht="34">
@@ -1126,16 +1210,16 @@
         <v>6</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="E19" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" ht="34">
@@ -1143,15 +1227,17 @@
         <v>7</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="E20" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="G20" s="9"/>
     </row>
@@ -1160,15 +1246,17 @@
         <v>8</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
+      <c r="D21" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="E21" s="9" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="G21" s="9"/>
     </row>
@@ -1177,16 +1265,16 @@
         <v>9</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
+      <c r="D22" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="E22" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7" ht="51">
@@ -1194,16 +1282,16 @@
         <v>10</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="E23" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>43</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" ht="34">
@@ -1211,19 +1299,21 @@
         <v>11</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
+      <c r="D24" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="E24" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7" ht="34">
+    <row r="25" spans="1:7" ht="17">
       <c r="A25" s="1">
         <v>12</v>
       </c>
@@ -1232,9 +1322,11 @@
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
+      <c r="E25" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="F25" s="9" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="G25" s="9"/>
     </row>
@@ -1247,10 +1339,10 @@
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="E26" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7">
@@ -1269,14 +1361,16 @@
         <v>1</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="D28" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7" ht="34">
@@ -1284,14 +1378,16 @@
         <v>2</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="D29" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7" ht="17">
@@ -1299,14 +1395,16 @@
         <v>3</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="D30" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
     <row r="31" spans="1:7" ht="34">
@@ -1314,28 +1412,32 @@
         <v>4</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="9"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" ht="34">
+    <row r="32" spans="1:7" ht="17">
       <c r="A32" s="1">
         <v>5</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="11"/>
+      <c r="D32" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="F32" s="9" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="G32" s="9"/>
     </row>
@@ -1344,71 +1446,71 @@
         <v>6</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="9"/>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" ht="68">
+    <row r="34" spans="1:7" ht="51">
       <c r="A34" s="1">
         <v>7</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="D34" s="11"/>
+      <c r="E34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="9"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" ht="90">
+    <row r="35" spans="1:7" ht="75">
       <c r="A35" s="1">
         <v>8</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="9"/>
       <c r="G35" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A5:G35">
-    <cfRule type="expression" dxfId="5" priority="10">
-      <formula>$F5=$I$7</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="11">
-      <formula>$F5=$I$6</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="13">
-      <formula>$F5=$I$5</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I5:I7">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>$I5=$I$7</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$I5=$I$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>$I5=$I$5</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F12 F14:F26 F28:F35" xr:uid="{9ECECD3F-B10C-D446-A358-3A7D162D644C}">
+  <conditionalFormatting sqref="A5:G35">
+    <cfRule type="expression" dxfId="2" priority="14">
+      <formula>$E5=$I$7</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="15">
+      <formula>$E5=$I$6</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="16">
+      <formula>$E5=$I$5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E12 E14:E26 E28:E35" xr:uid="{9ECECD3F-B10C-D446-A358-3A7D162D644C}">
       <formula1>$I$5:$I$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>